<commit_message>
Working on Msg delays. Saving one by one, but it would be a huge file... Checking the necessity to summary it before save.
</commit_message>
<xml_diff>
--- a/results/2017-03-24 - lotOfois/Stats - 2017-03-24.xlsx
+++ b/results/2017-03-24 - lotOfois/Stats - 2017-03-24.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="2505" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="3105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -719,7 +719,7 @@
             <c:numRef>
               <c:f>Sheet2!$D$26:$D$29</c:f>
               <c:numCache>
-                <c:formatCode>#.##00000</c:formatCode>
+                <c:formatCode>#,##0.0000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>7.46</c:v>
@@ -746,11 +746,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="137361120"/>
-        <c:axId val="137364256"/>
+        <c:axId val="132942960"/>
+        <c:axId val="132938256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="137361120"/>
+        <c:axId val="132942960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -804,12 +804,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="137364256"/>
+        <c:crossAx val="132938256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="137364256"/>
+        <c:axId val="132938256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -863,7 +863,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="137361120"/>
+        <c:crossAx val="132942960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1460,11 +1460,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="364319792"/>
-        <c:axId val="364320968"/>
+        <c:axId val="132938648"/>
+        <c:axId val="132939040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="364319792"/>
+        <c:axId val="132938648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1518,12 +1518,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364320968"/>
+        <c:crossAx val="132939040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="364320968"/>
+        <c:axId val="132939040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1577,7 +1577,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364319792"/>
+        <c:crossAx val="132938648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3130,8 +3130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S31" sqref="S31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3671,7 +3671,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D45" sqref="D45:D77"/>
     </sheetView>
   </sheetViews>

</xml_diff>